<commit_message>
modified main thesis boards and made changes to the GUI
</commit_message>
<xml_diff>
--- a/Finances/Order List 11-22-2013.xlsx
+++ b/Finances/Order List 11-22-2013.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Item</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>http://www.horizonhobby.com/products/receiver-pack-2500mah-6v-nimh-JRPB5006#t2</t>
+  </si>
+  <si>
+    <t>Arduino Due</t>
   </si>
 </sst>
 </file>
@@ -510,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,14 +599,14 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2">
         <v>49.99</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>49.99</v>
+        <v>99.98</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
@@ -638,7 +641,7 @@
         <v>9.99</v>
       </c>
       <c r="E9" s="2">
-        <f>C9*D9</f>
+        <f t="shared" ref="E9:E22" si="1">C9*D9</f>
         <v>9.99</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -656,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="2">
-        <f>C10*D10</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -674,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <f>C11*D11</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -692,7 +695,7 @@
         <v>5.25</v>
       </c>
       <c r="E12" s="2">
-        <f>C12*D12</f>
+        <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -710,7 +713,7 @@
         <v>19.95</v>
       </c>
       <c r="E13" s="2">
-        <f>C13*D13</f>
+        <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -728,7 +731,7 @@
         <v>14.95</v>
       </c>
       <c r="E14" s="2">
-        <f>C14*D14</f>
+        <f t="shared" si="1"/>
         <v>74.75</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -746,7 +749,7 @@
         <v>14.95</v>
       </c>
       <c r="E15" s="2">
-        <f>C15*D15</f>
+        <f t="shared" si="1"/>
         <v>59.8</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -764,7 +767,7 @@
         <v>149.99</v>
       </c>
       <c r="E16" s="2">
-        <f>C16*D16</f>
+        <f t="shared" si="1"/>
         <v>149.99</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -782,7 +785,7 @@
         <v>2.5</v>
       </c>
       <c r="E17" s="2">
-        <f>C17*D17</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -800,7 +803,7 @@
         <v>2.5</v>
       </c>
       <c r="E18" s="2">
-        <f>C18*D18</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -818,7 +821,7 @@
         <v>2.5</v>
       </c>
       <c r="E19" s="2">
-        <f>C19*D19</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -836,7 +839,7 @@
         <v>2.5</v>
       </c>
       <c r="E20" s="2">
-        <f>C20*D20</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -854,7 +857,7 @@
         <v>2.5</v>
       </c>
       <c r="E21" s="2">
-        <f>C21*D21</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -872,17 +875,22 @@
         <v>1.95</v>
       </c>
       <c r="E22" s="2">
-        <f>C22*D22</f>
+        <f t="shared" si="1"/>
         <v>9.75</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E26" s="3">
         <f>SUM(E4:E22)</f>
-        <v>869.98</v>
+        <v>919.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>